<commit_message>
[ENH] review change owner import template
</commit_message>
<xml_diff>
--- a/pabi_asset_management/xlsx_template/asset_changeowner.xlsx
+++ b/pabi_asset_management/xlsx_template/asset_changeowner.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Asset Change Owner</t>
   </si>
@@ -43,22 +43,28 @@
     <t xml:space="preserve">Building</t>
   </si>
   <si>
+    <t xml:space="preserve">Floor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Room</t>
   </si>
   <si>
-    <t xml:space="preserve">1202-001-0001-000000004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">101012</t>
+    <t xml:space="preserve">7110-006-0010-000000239</t>
   </si>
   <si>
     <t xml:space="preserve">001509</t>
   </si>
   <si>
-    <t xml:space="preserve">CO101</t>
+    <t xml:space="preserve">IN1</t>
   </si>
   <si>
-    <t xml:space="preserve">5975-009-0001-000000001</t>
+    <t xml:space="preserve">IN1-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN1-02-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">** Sample Line **</t>
   </si>
 </sst>
 </file>
@@ -279,20 +285,20 @@
   </sheetPr>
   <dimension ref="A1:AMG55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.5612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.1938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1021" min="7" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.48469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="7" style="1" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="8.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2343,15 +2349,16 @@
       <c r="AMF2" s="0"/>
       <c r="AMG2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
       <c r="B3" s="0"/>
       <c r="C3" s="0"/>
       <c r="D3" s="0"/>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="0"/>
+      <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="4" t="n">
+      <c r="G3" s="4" t="n">
         <v>43465</v>
       </c>
     </row>
@@ -2363,7 +2370,7 @@
       <c r="E4" s="0"/>
       <c r="F4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -2382,427 +2389,479 @@
       <c r="F5" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
         <v>9</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>101018</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="5" t="s">
+      <c r="E6" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>9</v>
+      <c r="G6" s="5" t="s">
+        <v>13</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="D7" s="6"/>
       <c r="E7" s="7"/>
-      <c r="F7" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
       <c r="F8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
       <c r="F9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
       <c r="F10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
       <c r="F11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
       <c r="F12" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
       <c r="F13" s="5"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
       <c r="F14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
       <c r="F15" s="5"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
       <c r="F16" s="5"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
       <c r="F17" s="5"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
       <c r="F18" s="5"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
       <c r="F19" s="5"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
       <c r="F20" s="5"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
       <c r="F21" s="5"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="7"/>
       <c r="F22" s="5"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>
       <c r="F23" s="5"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
       <c r="F24" s="5"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
       <c r="E25" s="7"/>
       <c r="F25" s="5"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="7"/>
       <c r="F26" s="5"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="7"/>
       <c r="F27" s="5"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="7"/>
       <c r="F28" s="5"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="7"/>
       <c r="F29" s="5"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="7"/>
       <c r="F30" s="5"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="7"/>
       <c r="F31" s="5"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="7"/>
       <c r="F32" s="5"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="7"/>
       <c r="F33" s="5"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="7"/>
       <c r="F34" s="5"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="7"/>
       <c r="F35" s="5"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="7"/>
       <c r="F36" s="5"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="7"/>
       <c r="F37" s="5"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="7"/>
       <c r="F38" s="5"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="7"/>
       <c r="F39" s="5"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="7"/>
       <c r="F40" s="5"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="7"/>
       <c r="F41" s="5"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="7"/>
       <c r="F42" s="5"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="7"/>
       <c r="F43" s="5"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="7"/>
       <c r="F44" s="5"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="7"/>
       <c r="F45" s="5"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="7"/>
       <c r="F46" s="5"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="7"/>
       <c r="F47" s="5"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="7"/>
       <c r="F48" s="5"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="7"/>
       <c r="F49" s="5"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="7"/>
       <c r="F50" s="5"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="7"/>
       <c r="F51" s="5"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G51" s="5"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="7"/>
       <c r="F52" s="5"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="7"/>
       <c r="F53" s="5"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="7"/>
       <c r="F54" s="5"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G54" s="5"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="7"/>
       <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[ENH] pabi_asset_management, add more dimension to asset change owner
:100755 100755 3a2863e8 b7a62095 M	pabi_asset_management/models/asset_changeowner.py
:100755 100755 3bb9aadf 3140cf1f M	pabi_asset_management/views/asset_changeowner_view.xml
</commit_message>
<xml_diff>
--- a/pabi_asset_management/xlsx_template/asset_changeowner.xlsx
+++ b/pabi_asset_management/xlsx_template/asset_changeowner.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Asset Change Owner</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t xml:space="preserve">Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invest Asset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Construction Phase</t>
   </si>
   <si>
     <t xml:space="preserve">Responsible By</t>
@@ -283,22 +289,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMG55"/>
+  <dimension ref="A1:AMI55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="7" style="1" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="8.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="11" style="1" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1325,6 +1335,8 @@
       <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
@@ -2348,6 +2360,8 @@
       <c r="AME2" s="0"/>
       <c r="AMF2" s="0"/>
       <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
@@ -2355,20 +2369,24 @@
       <c r="C3" s="0"/>
       <c r="D3" s="0"/>
       <c r="E3" s="0"/>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="I3" s="4" t="n">
         <v>43465</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
       <c r="B4" s="0"/>
       <c r="C4" s="0"/>
       <c r="D4" s="0"/>
       <c r="E4" s="0"/>
       <c r="F4" s="0"/>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
@@ -2392,471 +2410,577 @@
       <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="H5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" s="5" t="n">
         <v>101018</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="5" t="s">
         <v>14</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="7"/>
+      <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="7"/>
+      <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="7"/>
+      <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="7"/>
+      <c r="E30" s="5"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="7"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="7"/>
+      <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="7"/>
+      <c r="E33" s="5"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="7"/>
+      <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="E35" s="7"/>
+      <c r="E35" s="5"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="7"/>
+      <c r="E36" s="5"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="7"/>
+      <c r="E37" s="5"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="7"/>
+      <c r="E38" s="5"/>
       <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="7"/>
+      <c r="E39" s="5"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-      <c r="E40" s="7"/>
+      <c r="E40" s="5"/>
       <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
-      <c r="E41" s="7"/>
+      <c r="E41" s="5"/>
       <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
-      <c r="E42" s="7"/>
+      <c r="E42" s="5"/>
       <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
-      <c r="E43" s="7"/>
+      <c r="E43" s="5"/>
       <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="7"/>
+      <c r="E44" s="5"/>
       <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
-      <c r="E45" s="7"/>
+      <c r="E45" s="5"/>
       <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-      <c r="E46" s="7"/>
+      <c r="E46" s="5"/>
       <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
-      <c r="E47" s="7"/>
+      <c r="E47" s="5"/>
       <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
-      <c r="E48" s="7"/>
+      <c r="E48" s="5"/>
       <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
-      <c r="E49" s="7"/>
+      <c r="E49" s="5"/>
       <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
-      <c r="E50" s="7"/>
+      <c r="E50" s="5"/>
       <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
-      <c r="E51" s="7"/>
+      <c r="E51" s="5"/>
       <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
-      <c r="E52" s="7"/>
+      <c r="E52" s="5"/>
       <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
-      <c r="E53" s="7"/>
+      <c r="E53" s="5"/>
       <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="7"/>
+      <c r="E54" s="5"/>
       <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="7"/>
+      <c r="E55" s="5"/>
       <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>